<commit_message>
AE-1292 add missing tests
</commit_message>
<xml_diff>
--- a/tests/resources/example-001.xlsx
+++ b/tests/resources/example-001.xlsx
@@ -27,7 +27,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="13">
+  <fonts count="9">
     <font>
       <sz val="11.0"/>
       <color indexed="8"/>
@@ -75,28 +75,8 @@
       <sz val="11.0"/>
       <color indexed="8"/>
     </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <color indexed="8"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <color indexed="8"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <color indexed="8"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <color indexed="8"/>
-    </font>
   </fonts>
-  <fills count="14">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -130,26 +110,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6E0B4"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFE699"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF8CBAD"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF1BB90"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFF4B084"/>
       </patternFill>
     </fill>
@@ -176,7 +136,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFill="true" applyFont="true">
       <alignment wrapText="true"/>
@@ -190,31 +150,19 @@
     <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="0" applyFill="true" applyFont="true" applyAlignment="true">
       <alignment wrapText="false" textRotation="180" horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" xfId="0" applyFill="true" applyFont="true">
-      <alignment wrapText="false"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" xfId="0" applyFill="true" applyFont="true">
-      <alignment wrapText="false"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" xfId="0" applyFill="true" applyFont="true">
-      <alignment wrapText="false"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="0" xfId="0" applyFill="true" applyFont="true">
-      <alignment wrapText="false"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="0" xfId="0" applyFill="true" applyFont="true" applyAlignment="true">
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" xfId="0" applyFill="true" applyFont="true" applyAlignment="true">
       <alignment wrapText="false" textRotation="180" horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="11" borderId="0" xfId="0" applyFill="true" applyFont="true">
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" xfId="0" applyFill="true" applyFont="true">
       <alignment wrapText="false"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="12" borderId="0" xfId="0" applyFill="true" applyFont="true" applyAlignment="true">
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" xfId="0" applyFill="true" applyFont="true" applyAlignment="true">
       <alignment wrapText="false" textRotation="180" horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="13" borderId="0" xfId="0" applyFill="true" applyFont="true" applyAlignment="true">
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" xfId="0" applyFill="true" applyFont="true" applyAlignment="true">
       <alignment wrapText="false" textRotation="180" horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>

</xml_diff>